<commit_message>
add foundation and admin
</commit_message>
<xml_diff>
--- a/lab IP Planning.xlsx
+++ b/lab IP Planning.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vladek/Documents/lab/nutanix/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61F7C635-167F-6C48-BAF2-1CDD6DAC1787}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F1640B8-6720-FC40-9D6D-1E2B256E82B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="940" yWindow="660" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{7281F2C6-6647-E24F-8BE9-F1F23CAFF57D}"/>
+    <workbookView xWindow="940" yWindow="660" windowWidth="28040" windowHeight="17440" xr2:uid="{7281F2C6-6647-E24F-8BE9-F1F23CAFF57D}"/>
   </bookViews>
   <sheets>
     <sheet name="networks" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="136">
   <si>
     <t>host</t>
   </si>
@@ -87,9 +87,6 @@
     <t>n/a</t>
   </si>
   <si>
-    <t>10.8.1.0</t>
-  </si>
-  <si>
     <t>data bus</t>
   </si>
   <si>
@@ -99,12 +96,6 @@
     <t>ntnx-services</t>
   </si>
   <si>
-    <t>10.8.8.0</t>
-  </si>
-  <si>
-    <t>10.1.8.8</t>
-  </si>
-  <si>
     <t>services front end</t>
   </si>
   <si>
@@ -382,6 +373,78 @@
   </si>
   <si>
     <t>FS VM 3</t>
+  </si>
+  <si>
+    <t>k8s-1</t>
+  </si>
+  <si>
+    <t>10.1.8.100</t>
+  </si>
+  <si>
+    <t>k8s-1 VIP</t>
+  </si>
+  <si>
+    <t>foundation</t>
+  </si>
+  <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>10.1.8.110</t>
+  </si>
+  <si>
+    <t>10.1.8.111</t>
+  </si>
+  <si>
+    <t>Foundation VM</t>
+  </si>
+  <si>
+    <t>admin station</t>
+  </si>
+  <si>
+    <t>10.1.7.0</t>
+  </si>
+  <si>
+    <t>10.1.6.0</t>
+  </si>
+  <si>
+    <t>vms1</t>
+  </si>
+  <si>
+    <t>vms segment 1</t>
+  </si>
+  <si>
+    <t>10.1.6.1</t>
+  </si>
+  <si>
+    <t>10.1.21.0</t>
+  </si>
+  <si>
+    <t>10.1.21.1</t>
+  </si>
+  <si>
+    <t>vms2</t>
+  </si>
+  <si>
+    <t>vms3</t>
+  </si>
+  <si>
+    <t>vms segment 2</t>
+  </si>
+  <si>
+    <t>vms segment 3</t>
+  </si>
+  <si>
+    <t>10.1.22.1</t>
+  </si>
+  <si>
+    <t>10.1.23.1</t>
+  </si>
+  <si>
+    <t>10.1.22.0</t>
+  </si>
+  <si>
+    <t>10.1.23.0</t>
   </si>
 </sst>
 </file>
@@ -807,19 +870,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FEDEF03-81BE-534C-B3E2-CF7C90128E50}">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="4.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="4.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="16384" width="10.83203125" style="1"/>
@@ -868,7 +931,7 @@
         <v>10</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -876,7 +939,7 @@
         <v>13</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>16</v>
+        <v>121</v>
       </c>
       <c r="C3" s="2">
         <v>24</v>
@@ -888,18 +951,18 @@
         <v>15</v>
       </c>
       <c r="F3" s="2">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>20</v>
+        <v>122</v>
       </c>
       <c r="C4" s="2">
         <v>24</v>
@@ -908,26 +971,96 @@
         <v>10</v>
       </c>
       <c r="E4" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="F4" s="2">
+        <v>12</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="C5" s="2">
+        <v>24</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="F5" s="2">
         <v>21</v>
       </c>
-      <c r="F4" s="2">
+      <c r="G5" s="2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="C6" s="2">
+        <v>24</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="E6" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="F6" s="2">
         <v>22</v>
       </c>
+      <c r="G6" s="2" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="C7" s="2">
+        <v>24</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="F7" s="2">
+        <v>23</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>131</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFF25265-0902-BE42-B748-1DCD2E4232F7}">
-  <dimension ref="A1:D45"/>
+  <dimension ref="A1:D50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -971,32 +1104,32 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B4" s="2" t="str">
         <f>CONCATENATE(A4,".nutanix.lab")</f>
         <v>ns1.nutanix.lab</v>
       </c>
       <c r="C4" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>84</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B5" s="2" t="str">
         <f>CONCATENATE(A5,".nutanix.lab")</f>
         <v>ns2.nutanix.lab</v>
       </c>
       <c r="C5" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>85</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -1007,453 +1140,453 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>23</v>
+        <v>115</v>
       </c>
       <c r="B7" s="2" t="str">
         <f>CONCATENATE(A7,".nutanix.lab")</f>
-        <v>ipmi-ahv1.nutanix.lab</v>
+        <v>foundation.nutanix.lab</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>24</v>
+        <v>117</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>25</v>
+        <v>119</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>26</v>
+        <v>116</v>
       </c>
       <c r="B8" s="2" t="str">
         <f>CONCATENATE(A8,".nutanix.lab")</f>
-        <v>ipmi-ahv2.nutanix.lab</v>
+        <v>admin.nutanix.lab</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>29</v>
+        <v>118</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>32</v>
+        <v>120</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B9" s="2" t="str">
-        <f>CONCATENATE(A9,".nutanix.lab")</f>
-        <v>ipmi-ahv3.nutanix.lab</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>33</v>
-      </c>
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="B10" s="2" t="str">
         <f>CONCATENATE(A10,".nutanix.lab")</f>
-        <v>ipmi-ahv4.nutanix.lab</v>
+        <v>ipmi-ahv1.nutanix.lab</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
+      <c r="A11" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="2" t="str">
+        <f>CONCATENATE(A11,".nutanix.lab")</f>
+        <v>ipmi-ahv2.nutanix.lab</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="B12" s="2" t="str">
         <f>CONCATENATE(A12,".nutanix.lab")</f>
-        <v>ntnx-ahv1.nutanix.lab</v>
+        <v>ipmi-ahv3.nutanix.lab</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="B13" s="2" t="str">
         <f>CONCATENATE(A13,".nutanix.lab")</f>
-        <v>ntnx-ahv2.nutanix.lab</v>
+        <v>ipmi-ahv4.nutanix.lab</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B14" s="2" t="str">
-        <f>CONCATENATE(A14,".nutanix.lab")</f>
-        <v>ntnx-ahv3.nutanix.lab</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>46</v>
-      </c>
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B15" s="2" t="str">
         <f>CONCATENATE(A15,".nutanix.lab")</f>
-        <v>ntnx-ahv4.nutanix.lab</v>
+        <v>ntnx-ahv1.nutanix.lab</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="2"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
+      <c r="A16" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B16" s="2" t="str">
+        <f>CONCATENATE(A16,".nutanix.lab")</f>
+        <v>ntnx-ahv2.nutanix.lab</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="B17" s="4" t="str">
+      <c r="A17" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" s="2" t="str">
         <f>CONCATENATE(A17,".nutanix.lab")</f>
-        <v>ntnx-cluster1.nutanix.lab</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>60</v>
+        <v>ntnx-ahv3.nutanix.lab</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>61</v>
+        <v>43</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>55</v>
+        <v>35</v>
       </c>
       <c r="B18" s="2" t="str">
         <f>CONCATENATE(A18,".nutanix.lab")</f>
-        <v>ntnx-cvm1.nutanix.lab</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>51</v>
+        <v>ntnx-ahv4.nutanix.lab</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>39</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="2" t="s">
+      <c r="A19" s="2"/>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="B19" s="2" t="str">
-        <f>CONCATENATE(A19,".nutanix.lab")</f>
-        <v>ntnx-cvm2.nutanix.lab</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="2" t="s">
+      <c r="B20" s="4" t="str">
+        <f>CONCATENATE(A20,".nutanix.lab")</f>
+        <v>ntnx-cluster1.nutanix.lab</v>
+      </c>
+      <c r="C20" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="B20" s="2" t="str">
-        <f>CONCATENATE(A20,".nutanix.lab")</f>
-        <v>ntnx-cvm3.nutanix.lab</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>53</v>
-      </c>
       <c r="D20" s="2" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="B21" s="2" t="str">
         <f>CONCATENATE(A21,".nutanix.lab")</f>
+        <v>ntnx-cvm1.nutanix.lab</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B22" s="2" t="str">
+        <f>CONCATENATE(A22,".nutanix.lab")</f>
+        <v>ntnx-cvm2.nutanix.lab</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B23" s="2" t="str">
+        <f>CONCATENATE(A23,".nutanix.lab")</f>
+        <v>ntnx-cvm3.nutanix.lab</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B24" s="2" t="str">
+        <f>CONCATENATE(A24,".nutanix.lab")</f>
         <v>ntnx-cvm4.nutanix.lab</v>
       </c>
-      <c r="C21" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" s="2"/>
-      <c r="B22" s="2"/>
-      <c r="C22" s="2" t="s">
+      <c r="C24" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" s="2"/>
+      <c r="B25" s="2"/>
+      <c r="C25" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" s="2"/>
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B27" s="4" t="str">
+        <f>CONCATENATE(A27,".nutanix.lab")</f>
+        <v>ntnx-pc.nutanix.lab</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="D22" s="2" t="s">
+      <c r="B28" s="2" t="str">
+        <f>CONCATENATE(A28,".nutanix.lab")</f>
+        <v>ntnx-pc1.nutanix.lab</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" s="2" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" s="2"/>
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="B24" s="4" t="str">
-        <f>CONCATENATE(A24,".nutanix.lab")</f>
-        <v>ntnx-pc.nutanix.lab</v>
-      </c>
-      <c r="C24" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="B25" s="2" t="str">
-        <f>CONCATENATE(A25,".nutanix.lab")</f>
-        <v>ntnx-pc1.nutanix.lab</v>
-      </c>
-      <c r="C25" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="B26" s="2" t="str">
-        <f>CONCATENATE(A26,".nutanix.lab")</f>
+      <c r="B29" s="2" t="str">
+        <f>CONCATENATE(A29,".nutanix.lab")</f>
         <v>ntnx-pc2.nutanix.lab</v>
       </c>
-      <c r="C26" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27" s="2" t="s">
+      <c r="C29" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="D29" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="B27" s="2" t="str">
-        <f>CONCATENATE(A27,".nutanix.lab")</f>
-        <v>ntnx-pc3.nutanix.lab</v>
-      </c>
-      <c r="C27" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" s="2"/>
-      <c r="B28" s="2"/>
-      <c r="C28" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29" s="2"/>
-      <c r="B29" s="2"/>
-      <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
-        <v>106</v>
+        <v>64</v>
       </c>
       <c r="B30" s="2" t="str">
         <f>CONCATENATE(A30,".nutanix.lab")</f>
+        <v>ntnx-pc3.nutanix.lab</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" s="2"/>
+      <c r="B31" s="2"/>
+      <c r="C31" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" s="2"/>
+      <c r="B32" s="2"/>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B33" s="2" t="str">
+        <f>CONCATENATE(A33,".nutanix.lab")</f>
         <v>NTNX-fs-1.nutanix.lab</v>
       </c>
-      <c r="C30" s="7" t="s">
+      <c r="C33" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="B34" s="2" t="str">
+        <f t="shared" ref="B34:B35" si="0">CONCATENATE(A34,".nutanix.lab")</f>
+        <v>NTNX-fs-2.nutanix.lab</v>
+      </c>
+      <c r="C34" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="D30" s="2" t="s">
+      <c r="D34" s="2" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A31" s="2" t="s">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="B31" s="2" t="str">
-        <f t="shared" ref="B31:B32" si="0">CONCATENATE(A31,".nutanix.lab")</f>
-        <v>NTNX-fs-2.nutanix.lab</v>
-      </c>
-      <c r="C31" s="7" t="s">
-        <v>110</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A32" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="B32" s="2" t="str">
+      <c r="B35" s="2" t="str">
         <f t="shared" si="0"/>
         <v>NTNX-fs-3.nutanix.lab</v>
       </c>
-      <c r="C32" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A33" s="2"/>
-      <c r="B33" s="2"/>
-      <c r="C33" s="2"/>
-      <c r="D33" s="2"/>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A34" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="B34" s="4" t="str">
-        <f>CONCATENATE(A34,".nutanix.lab")</f>
-        <v>s3.nutanix.lab</v>
-      </c>
-      <c r="C34" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A35" s="2"/>
-      <c r="B35" s="2"/>
-      <c r="C35" s="5" t="s">
-        <v>94</v>
+      <c r="C35" s="7" t="s">
+        <v>110</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>98</v>
+        <v>111</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" s="2"/>
       <c r="B36" s="2"/>
-      <c r="C36" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>99</v>
-      </c>
+      <c r="C36" s="2"/>
+      <c r="D36" s="2"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A37" s="2"/>
-      <c r="B37" s="2"/>
+      <c r="A37" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="B37" s="4" t="str">
+        <f>CONCATENATE(A37,".nutanix.lab")</f>
+        <v>s3.nutanix.lab</v>
+      </c>
       <c r="C37" s="5" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" s="2"/>
       <c r="B38" s="2"/>
-      <c r="C38" s="2" t="s">
-        <v>102</v>
+      <c r="C38" s="5" t="s">
+        <v>91</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" s="2"/>
       <c r="B39" s="2"/>
-      <c r="C39" s="2" t="s">
-        <v>103</v>
+      <c r="C39" s="5" t="s">
+        <v>92</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" s="2"/>
       <c r="B40" s="2"/>
-      <c r="C40" s="2"/>
-      <c r="D40" s="2"/>
+      <c r="C40" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A41" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="B41" s="2" t="str">
-        <f>CONCATENATE(A41,".nutanix.lab")</f>
-        <v>sw-qfx-10g.nutanix.lab</v>
-      </c>
+      <c r="A41" s="2"/>
+      <c r="B41" s="2"/>
       <c r="C41" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="D41" s="6" t="s">
-        <v>86</v>
+        <v>99</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A42" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="B42" s="2" t="str">
-        <f>CONCATENATE(A42,".nutanix.lab")</f>
-        <v>sw-ex-1g.nutanix.lab</v>
-      </c>
+      <c r="A42" s="2"/>
+      <c r="B42" s="2"/>
       <c r="C42" s="2" t="s">
-        <v>75</v>
+        <v>100</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>76</v>
+        <v>102</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
@@ -1463,23 +1596,80 @@
       <c r="D43" s="2"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A44" s="2"/>
-      <c r="B44" s="2"/>
+      <c r="A44" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="B44" s="2" t="str">
+        <f t="shared" ref="B44" si="1">CONCATENATE(A44,".nutanix.lab")</f>
+        <v>k8s-1.nutanix.lab</v>
+      </c>
       <c r="C44" s="2" t="s">
-        <v>89</v>
+        <v>113</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>91</v>
+        <v>114</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" s="2"/>
       <c r="B45" s="2"/>
-      <c r="C45" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="D45" s="2" t="s">
-        <v>92</v>
+      <c r="C45" s="2"/>
+      <c r="D45" s="2"/>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A46" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B46" s="2" t="str">
+        <f>CONCATENATE(A46,".nutanix.lab")</f>
+        <v>sw-qfx-10g.nutanix.lab</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D46" s="6" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A47" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B47" s="2" t="str">
+        <f>CONCATENATE(A47,".nutanix.lab")</f>
+        <v>sw-ex-1g.nutanix.lab</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A48" s="2"/>
+      <c r="B48" s="2"/>
+      <c r="C48" s="2"/>
+      <c r="D48" s="2"/>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A49" s="2"/>
+      <c r="B49" s="2"/>
+      <c r="C49" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A50" s="2"/>
+      <c r="B50" s="2"/>
+      <c r="C50" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>89</v>
       </c>
     </row>
   </sheetData>

</xml_diff>